<commit_message>
Committing progress on lab 6
</commit_message>
<xml_diff>
--- a/335Lab/Lab 6/data/data1500.xlsx
+++ b/335Lab/Lab 6/data/data1500.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClassWork\ME335\335Lab\Lab 6\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Class Work\Current\ME335\335Lab\Lab 6\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243429D0-4736-4623-BF0F-F3E36603EDC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17837A51-A0B7-486B-AB20-E840A8B3AA93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" xr2:uid="{CF034567-C82D-4548-8DCF-A2412C8E9973}"/>
+    <workbookView xWindow="-28800" yWindow="2295" windowWidth="23040" windowHeight="12210" xr2:uid="{CF034567-C82D-4548-8DCF-A2412C8E9973}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>deltaP_inH20</t>
   </si>
@@ -40,6 +49,18 @@
   </si>
   <si>
     <t>valveSetting</t>
+  </si>
+  <si>
+    <t>motorActual_SD_RPM</t>
+  </si>
+  <si>
+    <t>deltaP_SD_inH20</t>
+  </si>
+  <si>
+    <t>flow_SD_GPM</t>
+  </si>
+  <si>
+    <t>torque_SD_lbft</t>
   </si>
 </sst>
 </file>
@@ -82,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -90,7 +111,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,23 +425,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD987997-35C0-456C-917D-4704B7619C20}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -429,282 +453,398 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>100</v>
       </c>
       <c r="B2" s="2">
         <v>1546.606</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
+        <v>11.413600658863064</v>
+      </c>
+      <c r="D2" s="2">
         <v>107.02</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="1">
+        <v>0.28213471959331909</v>
+      </c>
+      <c r="F2" s="2">
         <v>24.28</v>
       </c>
-      <c r="E2" s="2">
+      <c r="G2" s="1">
+        <v>2.2360679774997418E-2</v>
+      </c>
+      <c r="H2" s="2">
         <v>0.48</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>80</v>
       </c>
       <c r="B3" s="2">
         <v>1549.2380000000001</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
+        <v>12.065832752031637</v>
+      </c>
+      <c r="D3" s="2">
         <v>112.03400000000001</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="1">
+        <v>0.31698580409854271</v>
+      </c>
+      <c r="F3" s="2">
         <v>22.59</v>
       </c>
-      <c r="E3" s="2">
+      <c r="G3" s="1">
+        <v>3.5355339059327126E-2</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.47199999999999998</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" s="1">
+        <v>4.4721359549995832E-3</v>
+      </c>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>60</v>
       </c>
       <c r="B4" s="2">
         <v>1548.3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
+        <v>12.072657122605611</v>
+      </c>
+      <c r="D4" s="2">
         <v>124.306</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="1">
+        <v>0.20144478151592998</v>
+      </c>
+      <c r="F4" s="2">
         <v>17.725999999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G4" s="1">
+        <v>2.1908902300207637E-2</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.44</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="1">
+        <v>6.2063353831181828E-17</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>40</v>
       </c>
       <c r="B5" s="2">
         <v>1551.2380000000001</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
+        <v>10.553135553000347</v>
+      </c>
+      <c r="D5" s="2">
         <v>137.21199999999999</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="1">
+        <v>0.3449202806446745</v>
+      </c>
+      <c r="F5" s="2">
         <v>8.6259999999999994</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G5" s="1">
+        <v>4.6151923036857168E-2</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.36</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>20</v>
       </c>
       <c r="B6" s="2">
         <v>1550.2339999999999</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
+        <v>10.857832656658454</v>
+      </c>
+      <c r="D6" s="2">
         <v>139.392</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="1">
+        <v>5.7183913821981874E-2</v>
+      </c>
+      <c r="F6" s="2">
         <v>3.2879999999999998</v>
       </c>
-      <c r="E6" s="2">
+      <c r="G6" s="1">
+        <v>1.6431676725155012E-2</v>
+      </c>
+      <c r="H6" s="2">
         <v>0.318</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="I6" s="1">
+        <v>4.4721359549995832E-3</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
       <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>